<commit_message>
first round of h4 sweeps
</commit_message>
<xml_diff>
--- a/h4_daemon_results/speedup.xlsx
+++ b/h4_daemon_results/speedup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="4260" windowWidth="46480" windowHeight="21000" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="3280" yWindow="4260" windowWidth="46480" windowHeight="21000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="H4-Results" sheetId="1" r:id="rId1"/>
@@ -499,35 +499,35 @@
     </textPr>
   </connection>
   <connection id="58" name="test" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="59" name="test1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="60" name="test2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="61" name="test3" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="62" name="test4" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -535,7 +535,7 @@
     </textPr>
   </connection>
   <connection id="63" name="test5" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/npcarter/Desktop/test.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -1442,11 +1442,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1260735872"/>
-        <c:axId val="1261032512"/>
+        <c:axId val="553490704"/>
+        <c:axId val="676402784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1260735872"/>
+        <c:axId val="553490704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36.0"/>
@@ -1493,7 +1493,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1523,6 +1522,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1556,13 +1556,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1261032512"/>
+        <c:crossAx val="676402784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="6.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1261032512"/>
+        <c:axId val="676402784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1607,7 +1607,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1670,7 +1669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1260735872"/>
+        <c:crossAx val="553490704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1774,7 +1773,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2155,11 +2153,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1260656288"/>
-        <c:axId val="1260658608"/>
+        <c:axId val="656129840"/>
+        <c:axId val="660583712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1260656288"/>
+        <c:axId val="656129840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1260658608"/>
+        <c:crossAx val="660583712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2210,7 +2208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1260658608"/>
+        <c:axId val="660583712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,7 +2258,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1260656288"/>
+        <c:crossAx val="656129840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3273,11 +3271,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1304906592"/>
-        <c:axId val="1304909136"/>
+        <c:axId val="660392912"/>
+        <c:axId val="660205520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1304906592"/>
+        <c:axId val="660392912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540.0"/>
@@ -3324,7 +3322,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3387,13 +3384,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1304909136"/>
+        <c:crossAx val="660205520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="36.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1304909136"/>
+        <c:axId val="660205520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3438,7 +3435,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3501,7 +3497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1304906592"/>
+        <c:crossAx val="660392912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5347,163 +5343,163 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_22" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_23" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_24" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_25" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp" connectionId="55" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_1" connectionId="56" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_2" connectionId="57" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_3" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="onenode" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_27" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_28" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_29" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_30" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_31" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_41" connectionId="49" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_42" connectionId="50" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_43" connectionId="52" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_44" connectionId="53" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_16" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="onecore" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="onenode" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_32" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_5" connectionId="63" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_33" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_4" connectionId="62" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_34" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_3" connectionId="61" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_4" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_2" connectionId="60" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_39" connectionId="47" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_1" connectionId="59" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_9" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test" connectionId="58" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_10" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_11" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_12" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_13" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_6" connectionId="54" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_14" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_15" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_40" connectionId="48" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_5" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_7" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_5" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_40" connectionId="48" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_15" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_14" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_13" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_12" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_11" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_10" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_9" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_39" connectionId="47" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_4" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_3" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_2" connectionId="57" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_1" connectionId="56" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp" connectionId="55" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_25" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_24" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_23" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_22" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_21" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_2" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_20" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_19" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_18" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_17" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_38" connectionId="46" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_37" connectionId="45" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable46.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_36" connectionId="44" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test" connectionId="58" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable47.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5511,71 +5507,71 @@
 </file>
 
 <file path=xl/queryTables/queryTable48.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_34" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_36" connectionId="44" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable49.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_33" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_37" connectionId="45" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_3" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="onecore_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable50.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_32" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_38" connectionId="46" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable51.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_16" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_17" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable52.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_44" connectionId="53" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_18" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable53.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_43" connectionId="52" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_19" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable54.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_42" connectionId="50" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_1" connectionId="59" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable55.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_41" connectionId="49" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_2" connectionId="60" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable56.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_31" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_3" connectionId="61" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable57.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_30" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_4" connectionId="62" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable58.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_29" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_5" connectionId="63" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable59.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_28" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_8" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_4" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_5" connectionId="51" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable60.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_27" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_26" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable61.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_26" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_20" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable62.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_8" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_21" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable63.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5583,15 +5579,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_5" connectionId="51" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_4" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="onecore_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_3" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_6" connectionId="54" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_2" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5859,7 +5855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY166"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="AE48" workbookViewId="0">
+    <sheetView topLeftCell="AE48" workbookViewId="0">
       <selection activeCell="AX50" sqref="AX50"/>
     </sheetView>
   </sheetViews>
@@ -28066,7 +28062,7 @@
         <v>36.723166764532081</v>
       </c>
       <c r="AL164">
-        <f t="shared" ref="AL164:AX164" si="31">AVERAGE(AL113:AL162)</f>
+        <f t="shared" ref="AL164:AS164" si="31">AVERAGE(AL113:AL162)</f>
         <v>67.325537504711335</v>
       </c>
       <c r="AM164" t="e">
@@ -28271,7 +28267,7 @@
         <v>37.600298161899744</v>
       </c>
       <c r="AL165">
-        <f t="shared" ref="AL165:AX165" si="33">MEDIAN(AL113:AL162)</f>
+        <f t="shared" ref="AL165:AS165" si="33">MEDIAN(AL113:AL162)</f>
         <v>70.2451862504887</v>
       </c>
       <c r="AM165" t="e">
@@ -28336,7 +28332,7 @@
         <v>0.22229577962581823</v>
       </c>
       <c r="C166">
-        <f t="shared" ref="C166:AK166" si="34">_xlfn.STDEV.P(C113:C162)</f>
+        <f t="shared" ref="C166:AJ166" si="34">_xlfn.STDEV.P(C113:C162)</f>
         <v>0.39815552136002269</v>
       </c>
       <c r="D166">
@@ -28541,7 +28537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY60"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AY3"/>
     </sheetView>
   </sheetViews>
@@ -29595,7 +29591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA311"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A253" workbookViewId="0">
+    <sheetView topLeftCell="A253" workbookViewId="0">
       <selection activeCell="A289" sqref="A289"/>
     </sheetView>
   </sheetViews>
@@ -45834,7 +45830,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
@@ -45851,7 +45847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF59"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="AH1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="BE53" sqref="BE53"/>
     </sheetView>
   </sheetViews>
@@ -56564,7 +56560,7 @@
         <v>255.00176870540002</v>
       </c>
       <c r="D58">
-        <f t="shared" ref="D58:BF59" si="34">$C$53</f>
+        <f t="shared" ref="D58:BF58" si="34">$C$53</f>
         <v>255.00176870540002</v>
       </c>
       <c r="E58">
@@ -57025,7 +57021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>